<commit_message>
individuos creados en alojamiento hotel, albergue, apartahotel y camping
</commit_message>
<xml_diff>
--- a/oferta instancias.xlsx
+++ b/oferta instancias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\UDLA\proyecto\ontologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7CA93F-0257-4E56-B6D2-9D678BA38CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0CB9B9-84A2-48E9-90BB-317037CB3CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14685" windowHeight="15585" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t>Dirección</t>
   </si>
@@ -119,18 +119,12 @@
     <t>Desayuno, Wi-Fi gratuito</t>
   </si>
   <si>
-    <t>Hostal Costa del Caribe</t>
-  </si>
-  <si>
     <t>Cocina, área de descanso al aire libre, sala de TV</t>
   </si>
   <si>
     <t>Servicios incluidos: Desayuno, Wi-Fi gratuito</t>
   </si>
   <si>
-    <t>EcoAlbergue Sierra Verde</t>
-  </si>
-  <si>
     <t>Dormitorios compartidos</t>
   </si>
   <si>
@@ -282,6 +276,15 @@
   </si>
   <si>
     <t>Alquiler de tiendas de campaña y sacos de dormir</t>
+  </si>
+  <si>
+    <t>Camping</t>
+  </si>
+  <si>
+    <t>Albergue Costa del Caribe</t>
+  </si>
+  <si>
+    <t>Albergue EcoAlbergue Sierra Verde</t>
   </si>
 </sst>
 </file>
@@ -764,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1607584-0049-4B71-8163-81589441D782}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,7 +937,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="13">
         <v>80000</v>
@@ -954,10 +957,10 @@
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="13">
         <v>85000</v>
@@ -969,18 +972,18 @@
         <v>24</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="13">
         <v>150000</v>
@@ -989,21 +992,21 @@
         <v>4.5</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="13">
         <v>90000</v>
@@ -1015,15 +1018,15 @@
         <v>24</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1046,21 +1049,21 @@
         <v>1</v>
       </c>
       <c r="E19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" s="13">
         <v>200000</v>
@@ -1072,18 +1075,18 @@
         <v>10</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="13">
         <v>300000</v>
@@ -1095,18 +1098,18 @@
         <v>15</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="13">
         <v>400000</v>
@@ -1118,18 +1121,18 @@
         <v>18</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" s="13">
         <v>200000</v>
@@ -1141,15 +1144,15 @@
         <v>12</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1172,21 +1175,21 @@
         <v>1</v>
       </c>
       <c r="E27" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C28" s="13">
         <v>40000</v>
@@ -1195,21 +1198,21 @@
         <v>4.7</v>
       </c>
       <c r="E28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="13">
         <v>30000</v>
@@ -1218,21 +1221,21 @@
         <v>4.5</v>
       </c>
       <c r="E29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="G29" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" s="13">
         <v>80000</v>
@@ -1241,21 +1244,21 @@
         <v>4.8</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C31" s="13">
         <v>30000</v>
@@ -1264,13 +1267,13 @@
         <v>4.3</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit creacion del archivo editable de la ontologia
</commit_message>
<xml_diff>
--- a/oferta instancias.xlsx
+++ b/oferta instancias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\UDLA\proyecto\ontologia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\UDLA\Gestion del conocimiento\Proyecto final\ontologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0CB9B9-84A2-48E9-90BB-317037CB3CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{133A435F-72B4-472F-A1CB-CB2645B1A2A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
   </bookViews>
@@ -297,7 +297,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +335,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF262626"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -402,12 +409,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -427,6 +428,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -768,44 +775,44 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="32.140625" style="5"/>
-    <col min="3" max="3" width="32.140625" style="13"/>
-    <col min="4" max="4" width="32.140625" style="14"/>
+    <col min="3" max="3" width="32.140625" style="11"/>
+    <col min="4" max="4" width="32.140625" style="12"/>
     <col min="5" max="16384" width="32.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:7" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -873,7 +880,7 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2">
@@ -890,15 +897,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
@@ -907,19 +914,19 @@
       <c r="B10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -939,10 +946,10 @@
       <c r="B12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>80000</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>4.3</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -962,10 +969,10 @@
       <c r="B13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>85000</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>4</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -985,10 +992,10 @@
       <c r="B14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>150000</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <v>4.5</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -1008,10 +1015,10 @@
       <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>90000</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>4.2</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -1025,15 +1032,15 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
@@ -1042,19 +1049,19 @@
       <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="10" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1065,10 +1072,10 @@
       <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="11">
         <v>200000</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <v>4.5999999999999996</v>
       </c>
       <c r="E20" s="5">
@@ -1088,10 +1095,10 @@
       <c r="B21" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="11">
         <v>300000</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="12">
         <v>4.4000000000000004</v>
       </c>
       <c r="E21" s="5">
@@ -1111,10 +1118,10 @@
       <c r="B22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>400000</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="12">
         <v>4.8</v>
       </c>
       <c r="E22" s="5">
@@ -1134,10 +1141,10 @@
       <c r="B23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="11">
         <v>200000</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>4.2</v>
       </c>
       <c r="E23" s="5">
@@ -1151,15 +1158,15 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -1168,19 +1175,19 @@
       <c r="B27" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="9" t="s">
+      <c r="F27" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="10" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1191,10 +1198,10 @@
       <c r="B28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="11">
         <v>40000</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="12">
         <v>4.7</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -1214,10 +1221,10 @@
       <c r="B29" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="11">
         <v>30000</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="12">
         <v>4.5</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -1237,10 +1244,10 @@
       <c r="B30" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="11">
         <v>80000</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="12">
         <v>4.8</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -1260,10 +1267,10 @@
       <c r="B31" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="11">
         <v>30000</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="12">
         <v>4.3</v>
       </c>
       <c r="E31" s="5" t="s">

</xml_diff>

<commit_message>
creacion de instancias hasta la clase restauracion-bar de vinos
</commit_message>
<xml_diff>
--- a/oferta instancias.xlsx
+++ b/oferta instancias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\UDLA\Gestion del conocimiento\Proyecto final\ontologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0F16C6-DF98-4504-A315-7B831AB5092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89218A-4595-4614-9EB9-9D0CDE760EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13590" yWindow="0" windowWidth="14595" windowHeight="11295" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
   <si>
     <t>Hotel Andinos Plaza Florencia</t>
   </si>
@@ -62,9 +62,6 @@
     <t>HOTEL</t>
   </si>
   <si>
-    <t xml:space="preserve">Servicios disponibles </t>
-  </si>
-  <si>
     <t>Hotel Caqueta Real HSC</t>
   </si>
   <si>
@@ -251,9 +248,6 @@
     <t>servicio_de_limpieza</t>
   </si>
   <si>
-    <t>tipo_parcela</t>
-  </si>
-  <si>
     <t>servicio_de_camping</t>
   </si>
   <si>
@@ -269,18 +263,12 @@
     <t>Complejo_turístico</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipos_de_alojamientos_disponibles </t>
-  </si>
-  <si>
     <t>tipo_instalaciones_y_actividades</t>
   </si>
   <si>
     <t>Glamping</t>
   </si>
   <si>
-    <t xml:space="preserve">servicios_disponibles </t>
-  </si>
-  <si>
     <t xml:space="preserve">experiencias_unicas </t>
   </si>
   <si>
@@ -291,6 +279,111 @@
   </si>
   <si>
     <t>Hostal</t>
+  </si>
+  <si>
+    <t>tipo_camping</t>
+  </si>
+  <si>
+    <t>Motel</t>
+  </si>
+  <si>
+    <t>acceso_directo_habitacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tarifas_por_horas </t>
+  </si>
+  <si>
+    <t>flexibilidad_horaria</t>
+  </si>
+  <si>
+    <t>Pención</t>
+  </si>
+  <si>
+    <t>Residencia</t>
+  </si>
+  <si>
+    <t>servicio_disponible</t>
+  </si>
+  <si>
+    <t>descuentos_estancia_prolongada</t>
+  </si>
+  <si>
+    <t>duracion_minima_de_estadia</t>
+  </si>
+  <si>
+    <t>Vivienda_de_uso_turístico</t>
+  </si>
+  <si>
+    <t>Tipos_de_alojamientos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipo_de_propiedad </t>
+  </si>
+  <si>
+    <t>Agencia_de_viajes</t>
+  </si>
+  <si>
+    <t>contacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sitio_web </t>
+  </si>
+  <si>
+    <t>licencia</t>
+  </si>
+  <si>
+    <t>destinos</t>
+  </si>
+  <si>
+    <t>Agencia_de_viajes_online</t>
+  </si>
+  <si>
+    <t>asistencia_en_línea</t>
+  </si>
+  <si>
+    <t>metodos_de_pago_aceptados</t>
+  </si>
+  <si>
+    <t>Operador_receptivo</t>
+  </si>
+  <si>
+    <t>servicios_locales</t>
+  </si>
+  <si>
+    <t>idiomas_ofrecidos</t>
+  </si>
+  <si>
+    <t>paquetes_turisticos_ofrecidos</t>
+  </si>
+  <si>
+    <t>experiencias_exclusivas</t>
+  </si>
+  <si>
+    <t>Turoperador</t>
+  </si>
+  <si>
+    <t>horario_de_apertura</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Bar_de_vinos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipos_de_bebidas </t>
+  </si>
+  <si>
+    <t>origen_bebidas</t>
+  </si>
+  <si>
+    <t>Cafetería</t>
+  </si>
+  <si>
+    <t>Especialidad de café</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ambiente </t>
   </si>
 </sst>
 </file>
@@ -303,7 +396,7 @@
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,10 +445,34 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="9"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -380,12 +497,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -417,13 +534,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -470,18 +624,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="10"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -818,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1607584-0049-4B71-8163-81589441D782}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,41 +1023,42 @@
     <col min="3" max="3" width="32.140625" style="9"/>
     <col min="4" max="4" width="32.140625" style="10"/>
     <col min="5" max="5" width="36.7109375" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="32.140625" style="4"/>
+    <col min="6" max="6" width="44.42578125" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="32.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="E2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,10 +1078,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,10 +1101,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -930,18 +1124,18 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <v>296000</v>
@@ -953,44 +1147,44 @@
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="E10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1004,10 +1198,10 @@
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2">
         <v>80000</v>
@@ -1016,21 +1210,21 @@
         <v>4.3</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G12" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2">
         <v>85000</v>
@@ -1039,21 +1233,21 @@
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2">
         <v>150000</v>
@@ -1062,21 +1256,21 @@
         <v>4.5</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G14" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="2">
         <v>90000</v>
@@ -1085,55 +1279,55 @@
         <v>4.2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="A18" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="C20" s="2">
         <v>200000</v>
@@ -1145,18 +1339,18 @@
         <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C21" s="2">
         <v>300000</v>
@@ -1168,18 +1362,18 @@
         <v>15</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C22" s="2">
         <v>400000</v>
@@ -1191,18 +1385,18 @@
         <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C23" s="2">
         <v>200000</v>
@@ -1214,50 +1408,50 @@
         <v>12</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="A26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="E27" s="6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>39</v>
       </c>
       <c r="C28" s="2">
         <v>40000</v>
@@ -1266,19 +1460,19 @@
         <v>4.7</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>41</v>
       </c>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>43</v>
       </c>
       <c r="C29" s="2">
         <v>30000</v>
@@ -1287,19 +1481,19 @@
         <v>4.5</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>46</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>47</v>
       </c>
       <c r="C30" s="2">
         <v>80000</v>
@@ -1308,19 +1502,19 @@
         <v>4.8</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="C31" s="2">
         <v>30000</v>
@@ -1329,41 +1523,41 @@
         <v>4.3</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
+      <c r="A34" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="E35" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1375,33 +1569,33 @@
       <c r="F36"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-    </row>
-    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C38" s="11" t="s">
+      <c r="D38" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>78</v>
+      <c r="E38" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,67 +1607,501 @@
       <c r="F39"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
+      <c r="A40" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>59</v>
-      </c>
       <c r="E41" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="D45" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+    </row>
+    <row r="49" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="B49" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D49" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F45" s="6" t="s">
+      <c r="E49" s="26" t="s">
         <v>83</v>
       </c>
+      <c r="F49" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="18"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F52"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="31" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G55" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="25"/>
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="27"/>
+      <c r="N61" s="27"/>
+      <c r="O61" s="27"/>
+      <c r="P61" s="27"/>
+      <c r="Q61" s="27"/>
+      <c r="R61" s="27"/>
+      <c r="S61" s="27"/>
+      <c r="T61" s="27"/>
+      <c r="U61" s="27"/>
+      <c r="V61" s="27"/>
+      <c r="W61" s="27"/>
+      <c r="X61" s="27"/>
+      <c r="Y61" s="27"/>
+      <c r="Z61" s="27"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+    </row>
+    <row r="64" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F64" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="G64" s="30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="18"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="67" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="G67" s="30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E68"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+    </row>
+    <row r="70" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G70" s="30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="18"/>
+    </row>
+    <row r="73" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F73" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G73" s="30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E74" s="20"/>
+    </row>
+    <row r="75" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E75" s="20"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="27"/>
+      <c r="H76" s="27"/>
+      <c r="I76" s="27"/>
+      <c r="J76" s="27"/>
+      <c r="K76" s="27"/>
+      <c r="L76" s="27"/>
+      <c r="M76" s="27"/>
+      <c r="N76" s="27"/>
+      <c r="O76" s="27"/>
+      <c r="P76" s="27"/>
+      <c r="Q76" s="27"/>
+      <c r="R76" s="27"/>
+      <c r="S76" s="27"/>
+      <c r="T76" s="27"/>
+      <c r="U76" s="27"/>
+      <c r="V76" s="27"/>
+      <c r="W76" s="27"/>
+      <c r="X76" s="27"/>
+      <c r="Y76" s="27"/>
+      <c r="Z76" s="27"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="18"/>
+      <c r="G78" s="18"/>
+    </row>
+    <row r="79" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E79" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F79" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="G79" s="34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C82" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F82" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="G82" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="33"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84"/>
+    </row>
+    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E85" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F85" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G85" s="22"/>
+    </row>
+    <row r="86" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="19">
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="A54:G54"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A44:F44"/>

</xml_diff>

<commit_message>
pre pull creacion de instancias numero 1
</commit_message>
<xml_diff>
--- a/oferta instancias.xlsx
+++ b/oferta instancias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\UDLA\Gestion del conocimiento\Proyecto final\ontologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E89218A-4595-4614-9EB9-9D0CDE760EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EE61ED-A755-4630-8897-AEC1B7BC0041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="146">
   <si>
     <t>Hotel Andinos Plaza Florencia</t>
   </si>
@@ -380,10 +380,100 @@
     <t>Cafetería</t>
   </si>
   <si>
-    <t>Especialidad de café</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ambiente </t>
+    <t>especialidades_de_café</t>
+  </si>
+  <si>
+    <t>Casa_de_comidas_para_llevar</t>
+  </si>
+  <si>
+    <t>menu_del_día</t>
+  </si>
+  <si>
+    <t>tiempo_espera_promedio</t>
+  </si>
+  <si>
+    <t>Cervecería</t>
+  </si>
+  <si>
+    <t>marcas_de_cerveza_disponibles</t>
+  </si>
+  <si>
+    <t>eventos_especiales</t>
+  </si>
+  <si>
+    <t>Chocolatería</t>
+  </si>
+  <si>
+    <t>Coctelería</t>
+  </si>
+  <si>
+    <t>Heladería</t>
+  </si>
+  <si>
+    <t>Mercado gastronómico</t>
+  </si>
+  <si>
+    <t>Pub</t>
+  </si>
+  <si>
+    <t>Restaurante</t>
+  </si>
+  <si>
+    <t>Sidrería</t>
+  </si>
+  <si>
+    <t>Taberna</t>
+  </si>
+  <si>
+    <t>Tetería</t>
+  </si>
+  <si>
+    <t>variedades_de_chocolate</t>
+  </si>
+  <si>
+    <t>postres_ofrecidos</t>
+  </si>
+  <si>
+    <t>toppings_disponibles</t>
+  </si>
+  <si>
+    <t>variedad_de_helado</t>
+  </si>
+  <si>
+    <t>puestos_disponibles</t>
+  </si>
+  <si>
+    <t>eventos_gastronomicos_programados</t>
+  </si>
+  <si>
+    <t>tipo_de_cocina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reserva_previa_requerida </t>
+  </si>
+  <si>
+    <t>temporada_de_la_sidra</t>
+  </si>
+  <si>
+    <t>especialidades_gastronomicas</t>
+  </si>
+  <si>
+    <t>tapas_ofrecidas</t>
+  </si>
+  <si>
+    <t>variedad_de_te</t>
+  </si>
+  <si>
+    <t>decoracion_tematica</t>
+  </si>
+  <si>
+    <t>especialidad_de_cocteles</t>
+  </si>
+  <si>
+    <t>tipos_de_ambiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tipos_de_ambiente </t>
   </si>
 </sst>
 </file>
@@ -577,7 +667,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -624,33 +714,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="10"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -675,6 +743,27 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1011,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1607584-0049-4B71-8163-81589441D782}">
-  <dimension ref="A1:Z86"/>
+  <dimension ref="A1:Z123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,15 +1117,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1048,7 +1137,7 @@
       <c r="C2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -1154,15 +1243,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1174,7 +1263,7 @@
       <c r="C10" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -1289,15 +1378,15 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1309,7 +1398,7 @@
       <c r="C19" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="32" t="s">
+      <c r="D19" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E19" s="6" t="s">
@@ -1415,14 +1504,14 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1435,7 +1524,7 @@
       <c r="C27" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -1446,7 +1535,7 @@
       </c>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>37</v>
       </c>
@@ -1531,14 +1620,14 @@
       <c r="G31"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -1550,7 +1639,7 @@
       <c r="C35" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E35" s="6" t="s">
@@ -1569,14 +1658,14 @@
       <c r="F36"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1588,7 +1677,7 @@
       <c r="C38" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E38" s="13" t="s">
@@ -1607,14 +1696,14 @@
       <c r="F39"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
@@ -1626,7 +1715,7 @@
       <c r="C41" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E41" s="6" t="s">
@@ -1637,14 +1726,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -1656,25 +1745,25 @@
       <c r="C45" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="32" t="s">
+      <c r="D45" s="24" t="s">
         <v>58</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F45" s="16" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="27"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
@@ -1686,24 +1775,24 @@
       <c r="C49" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D49" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E49" s="26" t="s">
+      <c r="D49" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="F49" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
       <c r="F51"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1716,24 +1805,24 @@
       <c r="C52" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D52" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E52" s="26" t="s">
+      <c r="D52" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>85</v>
       </c>
       <c r="F52"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
     </row>
     <row r="55" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -1745,27 +1834,27 @@
       <c r="C55" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E55" s="31" t="s">
+      <c r="D55" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="F55" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G55" s="30" t="s">
+      <c r="G55" s="22" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="25"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="30"/>
       <c r="F57"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1778,51 +1867,51 @@
       <c r="C58" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D58" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="E58" s="26" t="s">
+      <c r="D58" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" s="18" t="s">
         <v>93</v>
       </c>
       <c r="F58"/>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
-      <c r="G61" s="27"/>
-      <c r="H61" s="27"/>
-      <c r="I61" s="27"/>
-      <c r="J61" s="27"/>
-      <c r="K61" s="27"/>
-      <c r="L61" s="27"/>
-      <c r="M61" s="27"/>
-      <c r="N61" s="27"/>
-      <c r="O61" s="27"/>
-      <c r="P61" s="27"/>
-      <c r="Q61" s="27"/>
-      <c r="R61" s="27"/>
-      <c r="S61" s="27"/>
-      <c r="T61" s="27"/>
-      <c r="U61" s="27"/>
-      <c r="V61" s="27"/>
-      <c r="W61" s="27"/>
-      <c r="X61" s="27"/>
-      <c r="Y61" s="27"/>
-      <c r="Z61" s="27"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="21"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
+      <c r="N61" s="19"/>
+      <c r="O61" s="19"/>
+      <c r="P61" s="19"/>
+      <c r="Q61" s="19"/>
+      <c r="R61" s="19"/>
+      <c r="S61" s="19"/>
+      <c r="T61" s="19"/>
+      <c r="U61" s="19"/>
+      <c r="V61" s="19"/>
+      <c r="W61" s="19"/>
+      <c r="X61" s="19"/>
+      <c r="Y61" s="19"/>
+      <c r="Z61" s="19"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="18"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
@@ -1831,7 +1920,7 @@
       <c r="B64" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="32" t="s">
+      <c r="C64" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D64" s="11" t="s">
@@ -1840,22 +1929,22 @@
       <c r="E64" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F64" s="26" t="s">
+      <c r="F64" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="G64" s="30" t="s">
+      <c r="G64" s="22" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
     </row>
     <row r="67" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
@@ -1864,7 +1953,7 @@
       <c r="B67" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C67" s="32" t="s">
+      <c r="C67" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D67" s="11" t="s">
@@ -1873,10 +1962,10 @@
       <c r="E67" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F67" s="26" t="s">
+      <c r="F67" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G67" s="30" t="s">
+      <c r="G67" s="22" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1884,14 +1973,14 @@
       <c r="E68"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="18"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
@@ -1900,7 +1989,7 @@
       <c r="B70" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="32" t="s">
+      <c r="C70" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D70" s="11" t="s">
@@ -1909,22 +1998,22 @@
       <c r="E70" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F70" s="26" t="s">
+      <c r="F70" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G70" s="30" t="s">
+      <c r="G70" s="22" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="18" t="s">
+      <c r="A72" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
@@ -1933,7 +2022,7 @@
       <c r="B73" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C73" s="32" t="s">
+      <c r="C73" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D73" s="11" t="s">
@@ -1942,57 +2031,57 @@
       <c r="E73" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F73" s="26" t="s">
+      <c r="F73" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="G73" s="30" t="s">
+      <c r="G73" s="22" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E74" s="20"/>
+      <c r="E74" s="17"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E75" s="20"/>
+      <c r="E75" s="17"/>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="27"/>
-      <c r="C76" s="28"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="27"/>
-      <c r="H76" s="27"/>
-      <c r="I76" s="27"/>
-      <c r="J76" s="27"/>
-      <c r="K76" s="27"/>
-      <c r="L76" s="27"/>
-      <c r="M76" s="27"/>
-      <c r="N76" s="27"/>
-      <c r="O76" s="27"/>
-      <c r="P76" s="27"/>
-      <c r="Q76" s="27"/>
-      <c r="R76" s="27"/>
-      <c r="S76" s="27"/>
-      <c r="T76" s="27"/>
-      <c r="U76" s="27"/>
-      <c r="V76" s="27"/>
-      <c r="W76" s="27"/>
-      <c r="X76" s="27"/>
-      <c r="Y76" s="27"/>
-      <c r="Z76" s="27"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="L76" s="19"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+      <c r="O76" s="19"/>
+      <c r="P76" s="19"/>
+      <c r="Q76" s="19"/>
+      <c r="R76" s="19"/>
+      <c r="S76" s="19"/>
+      <c r="T76" s="19"/>
+      <c r="U76" s="19"/>
+      <c r="V76" s="19"/>
+      <c r="W76" s="19"/>
+      <c r="X76" s="19"/>
+      <c r="Y76" s="19"/>
+      <c r="Z76" s="19"/>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="18"/>
-      <c r="G78" s="18"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="27"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="27"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -2001,7 +2090,7 @@
       <c r="B79" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C79" s="32" t="s">
+      <c r="C79" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D79" s="11" t="s">
@@ -2010,32 +2099,32 @@
       <c r="E79" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F79" s="34" t="s">
+      <c r="F79" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G79" s="34" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="18" t="s">
+      <c r="G79" s="26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-    </row>
-    <row r="82" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="27"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="27"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="27"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C82" s="32" t="s">
+      <c r="C82" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D82" s="11" t="s">
@@ -2044,35 +2133,35 @@
       <c r="E82" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F82" s="34" t="s">
+      <c r="F82" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G82" s="34" t="s">
+      <c r="G82" s="26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A83" s="33"/>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="18" t="s">
+    <row r="83" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="25"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84"/>
-    </row>
-    <row r="85" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B84" s="27"/>
+      <c r="C84" s="27"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="27"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="27"/>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C85" s="32" t="s">
+      <c r="C85" s="24" t="s">
         <v>58</v>
       </c>
       <c r="D85" s="11" t="s">
@@ -2081,23 +2170,454 @@
       <c r="E85" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F85" s="34" t="s">
+      <c r="F85" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="G85" s="22"/>
-    </row>
-    <row r="86" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A86" s="33"/>
+      <c r="G85" s="26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="25"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C88" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E88" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F88" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="G88" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" s="27"/>
+      <c r="C90" s="27"/>
+      <c r="D90" s="27"/>
+      <c r="E90" s="27"/>
+      <c r="F90" s="27"/>
+      <c r="G90" s="27"/>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B91" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E91" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F91" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G91" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="B94" s="27"/>
+      <c r="C94" s="27"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="27"/>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C95" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E95" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F95" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G95" s="26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="H96" s="25"/>
+    </row>
+    <row r="97" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="H97" s="25"/>
+    </row>
+    <row r="98" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="33"/>
+    </row>
+    <row r="99" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E99" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F99" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="G99" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="H99" s="33"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H100"/>
+      <c r="I100"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B101" s="27"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
+      <c r="G101" s="27"/>
+      <c r="H101"/>
+      <c r="I101"/>
+    </row>
+    <row r="102" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E102" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F102" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="G102" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="H102"/>
+      <c r="I102"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H103"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" s="27"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
+      <c r="G104" s="27"/>
+      <c r="H104"/>
+    </row>
+    <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C105" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E105" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F105" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G105" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="H105"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H106"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B107" s="27"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107"/>
+    </row>
+    <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E108" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F108" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G108" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="H108"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H109"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B110" s="27"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="27"/>
+      <c r="G110" s="27"/>
+      <c r="H110"/>
+    </row>
+    <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D111" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E111" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F111" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="G111" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="H111"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H112"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A113" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113" s="27"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
+      <c r="G113" s="27"/>
+      <c r="H113"/>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E114" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F114" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="G114" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="H114"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H115"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B116" s="27"/>
+      <c r="C116" s="27"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+      <c r="F116" s="27"/>
+      <c r="G116" s="27"/>
+      <c r="H116"/>
+    </row>
+    <row r="117" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E117" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F117" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G117" s="26"/>
+      <c r="H117"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H118"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B119" s="27"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="27"/>
+      <c r="G119" s="27"/>
+      <c r="H119"/>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C120" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E120" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F120" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G120" s="26"/>
+      <c r="H120"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H121"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H122"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H123"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A69:F69"/>
+  <mergeCells count="30">
+    <mergeCell ref="A113:G113"/>
+    <mergeCell ref="A116:G116"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="A101:G101"/>
+    <mergeCell ref="A104:G104"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="A110:G110"/>
+    <mergeCell ref="A87:G87"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A94:G94"/>
     <mergeCell ref="A48:F48"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A57:E57"/>
@@ -2110,6 +2630,13 @@
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A69:F69"/>
+    <mergeCell ref="A84:G84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
pre pull avance realizado hasta negocio local, servicios financieros, cajero
</commit_message>
<xml_diff>
--- a/oferta instancias.xlsx
+++ b/oferta instancias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\FAMILIA DIAZ PENAGOS\Documents\Gestion del conocimiento\Proyecto_final\ontologia-turismo-v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB18E0DA-5E23-4512-A872-A39FAA91E703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC7FAC49-5F0A-4DFA-9A5F-377A8D1F05B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
+    <workbookView xWindow="10005" yWindow="180" windowWidth="18255" windowHeight="15555" activeTab="1" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,47 +627,47 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1020,14 +1020,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1" ht="42" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -1130,15 +1130,15 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:7" ht="15.75">
       <c r="A10" s="6" t="s">
@@ -1265,15 +1265,15 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" ht="15.75">
       <c r="A19" s="6" t="s">
@@ -1391,15 +1391,15 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="1:7" ht="31.5">
       <c r="A27" s="6" t="s">
@@ -1532,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F938E12-23D9-41A7-B31B-2163AE58284A}">
   <dimension ref="B5:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1548,426 +1548,426 @@
   </cols>
   <sheetData>
     <row r="5" spans="2:8">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="2:8" ht="36">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="57">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="22">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="22" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="57">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="22">
         <v>4.8</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="71.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="22">
         <v>4.3</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="57">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="22">
         <v>4.5</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="2:8" ht="36">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="18" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="42.75">
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="19">
         <v>5</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="42.75">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="19">
         <v>4.8</v>
       </c>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="42.75">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="19">
         <v>4.3</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="42.75">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="D19" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="19">
         <v>4.5</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="42.75">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="19">
         <v>4</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="24" spans="2:8">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
     </row>
     <row r="25" spans="2:8" ht="36">
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="H25" s="28" t="s">
+      <c r="H25" s="25" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="42.75">
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>131</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F26" s="24">
+      <c r="F26" s="22">
         <v>5</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="42.75">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27" s="22">
         <v>4.8</v>
       </c>
-      <c r="G27" s="24" t="s">
+      <c r="G27" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="42.75">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28" s="22">
         <v>4.3</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="42.75">
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F29" s="24">
+      <c r="F29" s="22">
         <v>4.5</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H29" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="42.75">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="24">
+      <c r="F30" s="22">
         <v>4</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="22" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prepull adelanto de esteven
</commit_message>
<xml_diff>
--- a/oferta instancias.xlsx
+++ b/oferta instancias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\UDLA\Gestion del conocimiento\Proyecto final\ontologia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07FAA0F-6A97-4745-B396-367345A530DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3298A75-6C7B-4100-AC25-107A6A58BC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32441DA4-4E56-4D58-BA55-909C80965E84}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="183">
   <si>
     <t>Hotel Andinos Plaza Florencia</t>
   </si>
@@ -495,6 +495,96 @@
   </si>
   <si>
     <t>tipo_de_cambio_ofrecido</t>
+  </si>
+  <si>
+    <t>Devolución_de_IVA</t>
+  </si>
+  <si>
+    <t>requisitos_para_la_devolución</t>
+  </si>
+  <si>
+    <t>plazo_para_la_devolución</t>
+  </si>
+  <si>
+    <t>servicios_ofrecidos</t>
+  </si>
+  <si>
+    <t>Oficina_bancaria</t>
+  </si>
+  <si>
+    <t>bancos_asociados</t>
+  </si>
+  <si>
+    <t>Servicio_médico</t>
+  </si>
+  <si>
+    <t>Farmacia</t>
+  </si>
+  <si>
+    <t>Hospital_privado</t>
+  </si>
+  <si>
+    <t>tipo_de_productos_disponibles</t>
+  </si>
+  <si>
+    <t>especialidades_medicas_disponibles</t>
+  </si>
+  <si>
+    <t>equipamiento_medico</t>
+  </si>
+  <si>
+    <t>Servicios_varios</t>
+  </si>
+  <si>
+    <t>Consigna_de_equipaje</t>
+  </si>
+  <si>
+    <t>tarifa_por_periodo_de _almacenamiento</t>
+  </si>
+  <si>
+    <t>Locutorio</t>
+  </si>
+  <si>
+    <t>tamaño_maximo_de_equipaje_permitido</t>
+  </si>
+  <si>
+    <t>tarifas_de_llamadas</t>
+  </si>
+  <si>
+    <t>Paquetería_y_mensajería</t>
+  </si>
+  <si>
+    <t>tiempo_de_entrega_estimado</t>
+  </si>
+  <si>
+    <t>empresas_de_mensajeria_asociadas</t>
+  </si>
+  <si>
+    <t>Peluquería</t>
+  </si>
+  <si>
+    <t>productos_utilizados</t>
+  </si>
+  <si>
+    <t>Taller_mecánico</t>
+  </si>
+  <si>
+    <t>especialidades</t>
+  </si>
+  <si>
+    <t>marcas_de_vehiculos_atendidas</t>
+  </si>
+  <si>
+    <t>Tintorería o lavandería</t>
+  </si>
+  <si>
+    <t>Tipo de servicios (lavado en seco, lavado de prendas delicadas, planchado, etc.)</t>
+  </si>
+  <si>
+    <t>Productos utilizados (detergentes especiales, suavizantes, etc.)</t>
+  </si>
+  <si>
+    <t>Tintorería_o_lavandería</t>
   </si>
 </sst>
 </file>
@@ -780,35 +870,35 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1146,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1607584-0049-4B71-8163-81589441D782}">
-  <dimension ref="A1:Z132"/>
+  <dimension ref="A1:Z172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F130" sqref="F130"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,21 +1247,21 @@
     <col min="1" max="2" width="32.140625" style="4"/>
     <col min="3" max="3" width="32.140625" style="9"/>
     <col min="4" max="4" width="32.140625" style="10"/>
-    <col min="5" max="5" width="40.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="48.140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="44.42578125" style="4" customWidth="1"/>
     <col min="7" max="16384" width="32.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" s="7" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1289,15 +1379,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1424,15 +1514,15 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28" t="s">
+      <c r="A18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1550,14 +1640,14 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1666,14 +1756,14 @@
       <c r="G31"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
@@ -1704,14 +1794,14 @@
       <c r="F36"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="28"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
@@ -1742,14 +1832,14 @@
       <c r="F39"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="37"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
@@ -1772,14 +1862,14 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="37"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
@@ -1802,14 +1892,14 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="28"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
@@ -1832,13 +1922,13 @@
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
       <c r="F51"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1860,15 +1950,15 @@
       <c r="F52"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="B54" s="28"/>
-      <c r="C54" s="28"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="28"/>
-      <c r="F54" s="28"/>
-      <c r="G54" s="28"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
     </row>
     <row r="55" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
@@ -1894,13 +1984,13 @@
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="30"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="31"/>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="34"/>
       <c r="F57"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -1950,14 +2040,14 @@
       <c r="Z61" s="19"/>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="28"/>
-      <c r="D63" s="28"/>
-      <c r="E63" s="28"/>
-      <c r="F63" s="28"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
@@ -1983,14 +2073,14 @@
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="28" t="s">
+      <c r="A66" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
     </row>
     <row r="67" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
@@ -2019,14 +2109,14 @@
       <c r="E68"/>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
@@ -2052,14 +2142,14 @@
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A72" s="28" t="s">
+      <c r="A72" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B72" s="28"/>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
@@ -2119,15 +2209,15 @@
       <c r="Z76" s="19"/>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A78" s="28" t="s">
+      <c r="A78" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B78" s="28"/>
-      <c r="C78" s="28"/>
-      <c r="D78" s="28"/>
-      <c r="E78" s="28"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="28"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
@@ -2153,15 +2243,15 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="28" t="s">
+      <c r="A81" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B81" s="28"/>
-      <c r="C81" s="28"/>
-      <c r="D81" s="28"/>
-      <c r="E81" s="28"/>
-      <c r="F81" s="28"/>
-      <c r="G81" s="28"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="37"/>
+      <c r="G81" s="37"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
@@ -2190,15 +2280,15 @@
       <c r="A83" s="25"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="37" t="s">
         <v>113</v>
       </c>
-      <c r="B84" s="28"/>
-      <c r="C84" s="28"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="28"/>
-      <c r="F84" s="28"/>
-      <c r="G84" s="28"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
     </row>
     <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -2227,15 +2317,15 @@
       <c r="A86" s="25"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B87" s="28"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
-      <c r="E87" s="28"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="28"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
     </row>
     <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
@@ -2261,15 +2351,15 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="28" t="s">
+      <c r="A90" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="B90" s="28"/>
-      <c r="C90" s="28"/>
-      <c r="D90" s="28"/>
-      <c r="E90" s="28"/>
-      <c r="F90" s="28"/>
-      <c r="G90" s="28"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="37"/>
+      <c r="G90" s="37"/>
     </row>
     <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
@@ -2295,15 +2385,15 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="28" t="s">
+      <c r="A94" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="28"/>
+      <c r="B94" s="37"/>
+      <c r="C94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
     </row>
     <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
@@ -2335,15 +2425,15 @@
       <c r="H97" s="25"/>
     </row>
     <row r="98" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A98" s="28" t="s">
+      <c r="A98" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="B98" s="28"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
-      <c r="G98" s="28"/>
+      <c r="B98" s="37"/>
+      <c r="C98" s="37"/>
+      <c r="D98" s="37"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
       <c r="H98" s="27"/>
     </row>
     <row r="99" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
@@ -2375,15 +2465,15 @@
       <c r="I100"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="28" t="s">
+      <c r="A101" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="28"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
-      <c r="G101" s="28"/>
+      <c r="B101" s="37"/>
+      <c r="C101" s="37"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
       <c r="H101"/>
       <c r="I101"/>
     </row>
@@ -2416,15 +2506,15 @@
       <c r="H103"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="28" t="s">
+      <c r="A104" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="B104" s="28"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="28"/>
+      <c r="B104" s="37"/>
+      <c r="C104" s="37"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
       <c r="H104"/>
     </row>
     <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2455,15 +2545,15 @@
       <c r="H106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="28" t="s">
+      <c r="A107" s="37" t="s">
         <v>125</v>
       </c>
-      <c r="B107" s="28"/>
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
-      <c r="E107" s="28"/>
-      <c r="F107" s="28"/>
-      <c r="G107" s="28"/>
+      <c r="B107" s="37"/>
+      <c r="C107" s="37"/>
+      <c r="D107" s="37"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
       <c r="H107"/>
     </row>
     <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2494,15 +2584,15 @@
       <c r="H109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="B110" s="28"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="28"/>
-      <c r="F110" s="28"/>
-      <c r="G110" s="28"/>
+      <c r="B110" s="37"/>
+      <c r="C110" s="37"/>
+      <c r="D110" s="37"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="37"/>
       <c r="H110"/>
     </row>
     <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2533,15 +2623,15 @@
       <c r="H112"/>
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A113" s="28" t="s">
+      <c r="A113" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B113" s="28"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
-      <c r="F113" s="28"/>
-      <c r="G113" s="28"/>
+      <c r="B113" s="37"/>
+      <c r="C113" s="37"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="37"/>
       <c r="H113"/>
     </row>
     <row r="114" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -2572,15 +2662,15 @@
       <c r="H115"/>
     </row>
     <row r="116" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="B116" s="28"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="28"/>
-      <c r="G116" s="28"/>
+      <c r="B116" s="37"/>
+      <c r="C116" s="37"/>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="37"/>
+      <c r="G116" s="37"/>
       <c r="H116"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -2609,15 +2699,15 @@
       <c r="H118"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A119" s="28" t="s">
+      <c r="A119" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B119" s="28"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="28"/>
-      <c r="E119" s="28"/>
-      <c r="F119" s="28"/>
-      <c r="G119" s="28"/>
+      <c r="B119" s="37"/>
+      <c r="C119" s="37"/>
+      <c r="D119" s="37"/>
+      <c r="E119" s="37"/>
+      <c r="F119" s="37"/>
+      <c r="G119" s="37"/>
       <c r="H119"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -2652,7 +2742,7 @@
       <c r="A123" s="19"/>
       <c r="B123" s="19"/>
       <c r="C123" s="20"/>
-      <c r="D123" s="36" t="s">
+      <c r="D123" s="30" t="s">
         <v>146</v>
       </c>
       <c r="E123" s="19"/>
@@ -2679,17 +2769,17 @@
       <c r="Z123" s="19"/>
     </row>
     <row r="125" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B125" s="34"/>
+      <c r="B125" s="28"/>
     </row>
     <row r="126" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A126" s="29" t="s">
+      <c r="A126" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="B126" s="30"/>
-      <c r="C126" s="30"/>
-      <c r="D126" s="30"/>
-      <c r="E126" s="30"/>
-      <c r="F126" s="31"/>
+      <c r="B126" s="33"/>
+      <c r="C126" s="33"/>
+      <c r="D126" s="33"/>
+      <c r="E126" s="33"/>
+      <c r="F126" s="34"/>
       <c r="G126"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -2705,7 +2795,7 @@
       <c r="D127" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E127" s="35" t="s">
+      <c r="E127" s="29" t="s">
         <v>148</v>
       </c>
       <c r="F127" s="26" t="s">
@@ -2713,17 +2803,17 @@
       </c>
       <c r="G127"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" s="29" t="s">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A129" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="B129" s="30"/>
-      <c r="C129" s="30"/>
-      <c r="D129" s="30"/>
-      <c r="E129" s="30"/>
-      <c r="F129" s="31"/>
-    </row>
-    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B129" s="33"/>
+      <c r="C129" s="33"/>
+      <c r="D129" s="33"/>
+      <c r="E129" s="33"/>
+      <c r="F129" s="34"/>
+    </row>
+    <row r="130" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>56</v>
       </c>
@@ -2736,21 +2826,446 @@
       <c r="D130" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E130" s="35" t="s">
+      <c r="E130" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="F130" s="37" t="s">
+      <c r="F130" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E131" s="17"/>
     </row>
-    <row r="132" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E132" s="17"/>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A132" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="B132" s="33"/>
+      <c r="C132" s="33"/>
+      <c r="D132" s="33"/>
+      <c r="E132" s="33"/>
+      <c r="F132" s="34"/>
+    </row>
+    <row r="133" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C133" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D133" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E133" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F133" s="31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A135" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="B135" s="33"/>
+      <c r="C135" s="33"/>
+      <c r="D135" s="33"/>
+      <c r="E135" s="33"/>
+      <c r="F135" s="34"/>
+    </row>
+    <row r="136" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C136" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E136" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F136" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E137"/>
+      <c r="F137"/>
+    </row>
+    <row r="138" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="19"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="20"/>
+      <c r="D138" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E138" s="19"/>
+      <c r="F138" s="19"/>
+      <c r="G138" s="19"/>
+      <c r="H138" s="19"/>
+      <c r="I138" s="19"/>
+      <c r="J138" s="19"/>
+      <c r="K138" s="19"/>
+      <c r="L138" s="19"/>
+      <c r="M138" s="19"/>
+      <c r="N138" s="19"/>
+      <c r="O138" s="19"/>
+      <c r="P138" s="19"/>
+      <c r="Q138" s="19"/>
+      <c r="R138" s="19"/>
+      <c r="S138" s="19"/>
+      <c r="T138" s="19"/>
+      <c r="U138" s="19"/>
+      <c r="V138" s="19"/>
+      <c r="W138" s="19"/>
+      <c r="X138" s="19"/>
+      <c r="Y138" s="19"/>
+      <c r="Z138" s="19"/>
+    </row>
+    <row r="139" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D139"/>
+      <c r="E139"/>
+    </row>
+    <row r="140" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D140"/>
+      <c r="E140"/>
+    </row>
+    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A141" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="B141" s="33"/>
+      <c r="C141" s="33"/>
+      <c r="D141" s="33"/>
+      <c r="E141" s="33"/>
+      <c r="F141" s="34"/>
+    </row>
+    <row r="142" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C142" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D142" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E142" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="F142" s="31"/>
+    </row>
+    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A144" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="B144" s="33"/>
+      <c r="C144" s="33"/>
+      <c r="D144" s="33"/>
+      <c r="E144" s="33"/>
+      <c r="F144" s="34"/>
+    </row>
+    <row r="145" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C145" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D145" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E145" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F145" s="31" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="147" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A147" s="19"/>
+      <c r="B147" s="19"/>
+      <c r="C147" s="20"/>
+      <c r="D147" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="E147" s="19"/>
+      <c r="F147" s="19"/>
+      <c r="G147" s="19"/>
+      <c r="H147" s="19"/>
+      <c r="I147" s="19"/>
+      <c r="J147" s="19"/>
+      <c r="K147" s="19"/>
+      <c r="L147" s="19"/>
+      <c r="M147" s="19"/>
+      <c r="N147" s="19"/>
+      <c r="O147" s="19"/>
+      <c r="P147" s="19"/>
+      <c r="Q147" s="19"/>
+      <c r="R147" s="19"/>
+      <c r="S147" s="19"/>
+      <c r="T147" s="19"/>
+      <c r="U147" s="19"/>
+      <c r="V147" s="19"/>
+      <c r="W147" s="19"/>
+      <c r="X147" s="19"/>
+      <c r="Y147" s="19"/>
+      <c r="Z147" s="19"/>
+    </row>
+    <row r="148" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E148"/>
+      <c r="F148"/>
+    </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A149" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B149" s="33"/>
+      <c r="C149" s="33"/>
+      <c r="D149" s="33"/>
+      <c r="E149" s="33"/>
+      <c r="F149" s="34"/>
+    </row>
+    <row r="150" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C150" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D150" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E150" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="F150" s="31" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A152" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B152" s="33"/>
+      <c r="C152" s="33"/>
+      <c r="D152" s="33"/>
+      <c r="E152" s="33"/>
+      <c r="F152" s="34"/>
+    </row>
+    <row r="153" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C153" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D153" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E153" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="F153" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="154" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E154"/>
+    </row>
+    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A155" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B155" s="33"/>
+      <c r="C155" s="33"/>
+      <c r="D155" s="33"/>
+      <c r="E155" s="33"/>
+      <c r="F155" s="34"/>
+    </row>
+    <row r="156" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C156" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D156" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E156" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="F156" s="31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="158" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A158" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B158" s="33"/>
+      <c r="C158" s="33"/>
+      <c r="D158" s="33"/>
+      <c r="E158" s="33"/>
+      <c r="F158" s="34"/>
+    </row>
+    <row r="159" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C159" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E159" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F159" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D160"/>
+      <c r="E160"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="B161" s="33"/>
+      <c r="C161" s="33"/>
+      <c r="D161" s="33"/>
+      <c r="E161" s="33"/>
+      <c r="F161" s="34"/>
+    </row>
+    <row r="162" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C162" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E162" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="F162" s="31" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="B164" s="33"/>
+      <c r="C164" s="33"/>
+      <c r="D164" s="33"/>
+      <c r="E164" s="33"/>
+      <c r="F164" s="34"/>
+    </row>
+    <row r="165" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C165" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D165" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E165" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F165" s="31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D166"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D167"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C170" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C171" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C172" s="9" t="s">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="42">
+    <mergeCell ref="A164:F164"/>
+    <mergeCell ref="A152:F152"/>
+    <mergeCell ref="A155:F155"/>
+    <mergeCell ref="A158:F158"/>
+    <mergeCell ref="A161:F161"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A135:F135"/>
+    <mergeCell ref="A141:F141"/>
+    <mergeCell ref="A144:F144"/>
+    <mergeCell ref="A149:F149"/>
+    <mergeCell ref="A84:G84"/>
+    <mergeCell ref="A113:G113"/>
+    <mergeCell ref="A116:G116"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="A101:G101"/>
+    <mergeCell ref="A104:G104"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="A110:G110"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A69:F69"/>
     <mergeCell ref="A126:F126"/>
     <mergeCell ref="A129:F129"/>
     <mergeCell ref="A1:G1"/>
@@ -2767,22 +3282,6 @@
     <mergeCell ref="A48:F48"/>
     <mergeCell ref="A51:E51"/>
     <mergeCell ref="A57:E57"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A66:F66"/>
-    <mergeCell ref="A69:F69"/>
-    <mergeCell ref="A84:G84"/>
-    <mergeCell ref="A113:G113"/>
-    <mergeCell ref="A116:G116"/>
-    <mergeCell ref="A119:G119"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="A101:G101"/>
-    <mergeCell ref="A104:G104"/>
-    <mergeCell ref="A107:G107"/>
-    <mergeCell ref="A110:G110"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>